<commit_message>
Initial handle images #15
</commit_message>
<xml_diff>
--- a/tests/fixtures/image.xlsx
+++ b/tests/fixtures/image.xlsx
@@ -19,16 +19,28 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+  <si>
+    <t xml:space="preserve">test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test2</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -44,6 +56,11 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -95,7 +112,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -104,7 +121,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -131,9 +156,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>169200</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>1080</xdr:rowOff>
+      <xdr:colOff>168840</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>163080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -147,7 +172,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="360" y="360"/>
-          <a:ext cx="168840" cy="163080"/>
+          <a:ext cx="168480" cy="162720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -162,15 +187,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>5040</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>-360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>798120</xdr:colOff>
+      <xdr:colOff>802800</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>152640</xdr:rowOff>
+      <xdr:rowOff>151920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -183,8 +208,82 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="812520" y="325080"/>
-          <a:ext cx="798120" cy="315000"/>
+          <a:off x="817560" y="324720"/>
+          <a:ext cx="797760" cy="314640"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>954360</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>157680</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1122840</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>157680</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Image 1" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId3"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2811600" y="320040"/>
+          <a:ext cx="168480" cy="162720"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>3960</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>360</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>172440</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>163080</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Image 1" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId4"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1861200" y="487800"/>
+          <a:ext cx="168480" cy="162720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -200,7 +299,48 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" guid="{70FFFFFF-FFFF-FFFF-0100-000000000000}"/>
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" guid="{F294315C-9521-4652-8D85-F0BD8E4FDBAE}">
+  <header guid="{F294315C-9521-4652-8D85-F0BD8E4FDBAE}" dateTime="2021-06-06T21:12:00.000000000Z" userName=" " r:id="rId1" minRId="1" maxRId="2" maxSheetId="2">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+</headers>
+</file>
+
+<file path=xl/revisions/revisionLog1.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rcc rId="1" ua="false" sId="1">
+    <nc r="C3" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">test</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="2" ua="false" sId="1">
+    <nc r="C4" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">test2</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
 </file>
 
 <file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
@@ -215,24 +355,28 @@
   <dimension ref="B3:C4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.96"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
+      <c r="C3" s="2" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="2"/>
-      <c r="C4" s="1"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="4" t="s">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>